<commit_message>
feat: habilitar ajustes, predicciones y despliegue railway (v3.0.7)
</commit_message>
<xml_diff>
--- a/outputs/resultado_optimizacion_gps_fase1.xlsx
+++ b/outputs/resultado_optimizacion_gps_fase1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,12 +463,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Antofagasta</t>
+          <t>Viña del Mar</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Orlando</t>
+          <t>Luis</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -477,33 +477,240 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>12.46700421940928</v>
+        <v>43.6863</v>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Chillán</t>
+          <t>Talca</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>Luis</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>terrestre</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>16.0235</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Antofagasta</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Orlando</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>terrestre</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>19.82393333333333</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Calama</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Orlando</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>terrestre</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>7.286666666666667</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Iquique</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Orlando</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>terrestre</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>10.33776666666667</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Temuco</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>Jimmy</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>terrestre</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>10.00965400843882</v>
-      </c>
-      <c r="E3" t="n">
-        <v>4</v>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>terrestre</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>25.81096666666667</v>
+      </c>
+      <c r="E7" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Concepcion</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Jimmy</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>terrestre</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>28.2453</v>
+      </c>
+      <c r="E8" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Chillan</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Jimmy</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>terrestre</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>9.950000000000001</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Puerto Montt</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Jimmy</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>terrestre</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>15.81144</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Osorno</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Jimmy</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>terrestre</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>16.268</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Jimmy</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>terrestre</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>14.5658</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>